<commit_message>
added tags and updated app
</commit_message>
<xml_diff>
--- a/Data/trackingSheet.xlsx
+++ b/Data/trackingSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22819"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\OICE_16_974FA576_32C1D314_177A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6b0b84a9b3242542/Sensing_Sytems/somnia/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{496F528E-A62A-4F13-BCF1-23C77EA08C20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2483" yWindow="2483" windowWidth="16874" windowHeight="10522" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -898,15 +898,16 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -932,7 +933,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -943,7 +944,7 @@
         <v>1586939742169</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -954,7 +955,7 @@
         <v>1586916190797</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>416</v>
       </c>
@@ -965,7 +966,7 @@
         <v>1587028916380</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>417</v>
       </c>
@@ -976,7 +977,7 @@
         <v>1587115911544</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>418</v>
       </c>
@@ -987,7 +988,7 @@
         <v>1587193574168</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>419</v>
       </c>
@@ -998,7 +999,7 @@
         <v>1587285953475</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>420</v>
       </c>

</xml_diff>

<commit_message>
added windows to app
</commit_message>
<xml_diff>
--- a/Data/trackingSheet.xlsx
+++ b/Data/trackingSheet.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{496F528E-A62A-4F13-BCF1-23C77EA08C20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2483" yWindow="2483" windowWidth="16874" windowHeight="10522" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -898,7 +898,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>